<commit_message>
no more b&b error
</commit_message>
<xml_diff>
--- a/30 s/Branch_and_cut_sol.xlsx
+++ b/30 s/Branch_and_cut_sol.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>nom_fichier</t>
   </si>
@@ -45,46 +45,100 @@
     <t>gap</t>
   </si>
   <si>
+    <t>                              </t>
+  </si>
+  <si>
+    <t>                                                                                                                                                                                                        </t>
+  </si>
+  <si>
     <t>10_ulysses_3.tsp</t>
   </si>
   <si>
-    <t>[1, 2, 3, 10][5, 9][4, 6, 7...</t>
+    <t>136.99527629589417</t>
+  </si>
+  <si>
+    <t>[5, 9][1, 2, 3, 10][4, 6, 7, 8]</t>
   </si>
   <si>
     <t>10_ulysses_6.tsp</t>
   </si>
   <si>
-    <t>[6, 9][5][10][1, 2][3, 8][4...</t>
+    <t>55.11939124322688</t>
+  </si>
+  <si>
+    <t>[10][6, 9][5][2, 3][1, 4, 8][7]</t>
   </si>
   <si>
     <t>10_ulysses_9.tsp</t>
   </si>
   <si>
-    <t>[6][5][9][7][1][2, 3][8][4]...</t>
+    <t>33.29189782877749</t>
+  </si>
+  <si>
+    <t>[6][5][9][7][1][2, 3][8][4][10]</t>
   </si>
   <si>
     <t>14_burma_3.tsp</t>
   </si>
   <si>
-    <t>[3, 4, 7, 8, 14][1, 5, 6, 1...</t>
+    <t>93.38998725996821</t>
+  </si>
+  <si>
+    <t>[3, 4, 5, 6, 7][1, 8, 9, 10, 11][2, 12, 13, 14]</t>
   </si>
   <si>
     <t>14_burma_6.tsp</t>
   </si>
   <si>
-    <t>[7][6, 12, 13][9, 10, 11][1...</t>
+    <t>43.129462546693226</t>
+  </si>
+  <si>
+    <t>[5, 10][7][2, 8][6, 12, 13][3, 4, 14][1, 9, 11]</t>
   </si>
   <si>
     <t>14_burma_9.tsp</t>
   </si>
   <si>
-    <t>[4][6, 12][2, 13][9, 10][8,...</t>
+    <t>20.762438566071065</t>
+  </si>
+  <si>
+    <t>[3, 4][9, 11][10][1, 8][7][5][13, 14][6, 12][2]</t>
   </si>
   <si>
     <t>22_ulysses_3.tsp</t>
   </si>
   <si>
-    <t>[2, 3, 4, 10, 13, 16, 17, 1...</t>
+    <t>515.5925785532522</t>
+  </si>
+  <si>
+    <t>[1, 2, 3, 7, 13, 16, 18, 22][5, 6, 9, 10, 12, 14, 21][4, 8, 11, 15, 17, 19, 20]</t>
+  </si>
+  <si>
+    <t>26_eil_3.tsp</t>
+  </si>
+  <si>
+    <t>3475.635504853873</t>
+  </si>
+  <si>
+    <t>[6, 9, 13, 14, 16, 17, 18, 26][2, 4, 7, 8, 12, 20, 21, 22, 24][1, 3, 5, 10, 11, 15, 19, 23, 25]</t>
+  </si>
+  <si>
+    <t>26_eil_6.tsp</t>
+  </si>
+  <si>
+    <t>1485.7858771055776</t>
+  </si>
+  <si>
+    <t>[4, 13, 19][2, 5, 6, 10, 20][1, 14, 15, 16, 17, 25][3, 11, 12, 22, 23][7, 8, 24, 26][9, 18, 21]</t>
+  </si>
+  <si>
+    <t>26_eil_9.tsp</t>
+  </si>
+  <si>
+    <t>1006.5109586516216</t>
+  </si>
+  <si>
+    <t>[3, 8, 18][22, 23, 25][5, 14, 17][1, 4, 15][6, 12, 13][10, 11, 21][2, 7, 20][19, 24][9, 16, 26]</t>
   </si>
 </sst>
 </file>
@@ -436,7 +490,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -467,16 +521,16 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.8469998836517334</v>
-      </c>
-      <c r="C2">
-        <v>136.99527629589417</v>
+        <v>0.0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2">
-        <v>136.99527629589417</v>
+        <v>0.0</v>
       </c>
       <c r="F2">
         <v>0.0</v>
@@ -487,56 +541,56 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>8.82800006866455</v>
-      </c>
-      <c r="C3">
-        <v>26.66976329399166</v>
+        <v>3.868</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>26.669388513548007</v>
+        <v>136.99420807981383</v>
       </c>
       <c r="F3">
-        <v>1.405263479547286e-5</v>
+        <v>7.797466520183073e-6</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>6.383000135421753</v>
-      </c>
-      <c r="C4">
-        <v>33.29189782877749</v>
+        <v>15.50600004196167</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E4">
-        <v>33.29189782877749</v>
+        <v>55.11442110891486</v>
       </c>
       <c r="F4">
-        <v>0.0</v>
+        <v>9.017034114322455e-5</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5">
-        <v>7.73799991607666</v>
-      </c>
-      <c r="C5">
-        <v>93.0112453952746</v>
+        <v>7.161999940872192</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E5">
-        <v>93.0112453952746</v>
+        <v>33.29189782877749</v>
       </c>
       <c r="F5">
         <v>0.0</v>
@@ -544,62 +598,142 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B6">
-        <v>30.013000011444092</v>
-      </c>
-      <c r="C6">
-        <v>29.132718633500858</v>
+        <v>4.638000011444092</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E6">
-        <v>0.0</v>
+        <v>93.38998725996821</v>
       </c>
       <c r="F6">
-        <v>0.9999999999965675</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B7">
-        <v>30.02300000190735</v>
-      </c>
-      <c r="C7">
-        <v>10.307782907492081</v>
+        <v>30.003999948501587</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E7">
         <v>0.0</v>
       </c>
       <c r="F7">
-        <v>0.9999999999902985</v>
+        <v>0.9999999999976814</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B8">
-        <v>30.020000219345093</v>
-      </c>
-      <c r="C8">
-        <v>440.41518319221746</v>
+        <v>30.026999950408936</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E8">
-        <v>153.39431360797954</v>
+        <v>0.0</v>
       </c>
       <c r="F8">
-        <v>0.6517052103058483</v>
+        <v>0.9999999999951837</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>30.028000116348267</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9">
+        <v>149.9123235516313</v>
+      </c>
+      <c r="F9">
+        <v>0.7092426660361273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10">
+        <v>30.0239999294281</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10">
+        <v>191.3265443301569</v>
+      </c>
+      <c r="F10">
+        <v>0.9449520687474116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11">
+        <v>30.049000024795532</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11">
+        <v>0.0</v>
+      </c>
+      <c r="F11">
+        <v>0.9999999999999327</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <v>30.031999826431274</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12">
+        <v>0.0</v>
+      </c>
+      <c r="F12">
+        <v>0.9999999999999006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit results and report
</commit_message>
<xml_diff>
--- a/30 s/Branch_and_cut_sol.xlsx
+++ b/30 s/Branch_and_cut_sol.xlsx
@@ -90,10 +90,10 @@
     <t>14_burma_6.tsp</t>
   </si>
   <si>
-    <t>43.129462546693226</t>
-  </si>
-  <si>
-    <t>[5, 10][7][2, 8][6, 12, 13][3, 4, 14][1, 9, 11]</t>
+    <t>42.740623542601746</t>
+  </si>
+  <si>
+    <t>[7][6, 12, 14][2, 13][3, 4, 5][9, 10][1, 8, 11]</t>
   </si>
   <si>
     <t>14_burma_9.tsp</t>
@@ -108,10 +108,10 @@
     <t>22_ulysses_3.tsp</t>
   </si>
   <si>
-    <t>515.5925785532522</t>
-  </si>
-  <si>
-    <t>[1, 2, 3, 7, 13, 16, 18, 22][5, 6, 9, 10, 12, 14, 21][4, 8, 11, 15, 17, 19, 20]</t>
+    <t>414.58990456431127</t>
+  </si>
+  <si>
+    <t>[5, 6, 7, 13, 14, 15, 18][1, 2, 3, 4, 8, 16, 17, 20, 22][9, 10, 11, 12, 19, 21]</t>
   </si>
   <si>
     <t>26_eil_3.tsp</t>
@@ -541,7 +541,7 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>3.868</v>
+        <v>2.509000062942505</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -561,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>15.50600004196167</v>
+        <v>20.182999849319458</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -581,7 +581,7 @@
         <v>14</v>
       </c>
       <c r="B5">
-        <v>7.161999940872192</v>
+        <v>10.39300012588501</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -601,7 +601,7 @@
         <v>17</v>
       </c>
       <c r="B6">
-        <v>4.638000011444092</v>
+        <v>3.1100001335144043</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -621,7 +621,7 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <v>30.003999948501587</v>
+        <v>30.019999980926514</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -633,7 +633,7 @@
         <v>0.0</v>
       </c>
       <c r="F7">
-        <v>0.9999999999976814</v>
+        <v>0.9999999999976603</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -641,7 +641,7 @@
         <v>23</v>
       </c>
       <c r="B8">
-        <v>30.026999950408936</v>
+        <v>30.013999938964844</v>
       </c>
       <c r="C8" t="s">
         <v>24</v>
@@ -661,7 +661,7 @@
         <v>26</v>
       </c>
       <c r="B9">
-        <v>30.028000116348267</v>
+        <v>30.017000198364258</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
@@ -670,10 +670,10 @@
         <v>28</v>
       </c>
       <c r="E9">
-        <v>149.9123235516313</v>
+        <v>173.61775574493146</v>
       </c>
       <c r="F9">
-        <v>0.7092426660361273</v>
+        <v>0.5812301413189429</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -681,7 +681,7 @@
         <v>29</v>
       </c>
       <c r="B10">
-        <v>30.0239999294281</v>
+        <v>30.027000188827515</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
@@ -690,10 +690,10 @@
         <v>31</v>
       </c>
       <c r="E10">
-        <v>191.3265443301569</v>
+        <v>177.98397630890767</v>
       </c>
       <c r="F10">
-        <v>0.9449520687474116</v>
+        <v>0.9487909546152236</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -701,7 +701,7 @@
         <v>32</v>
       </c>
       <c r="B11">
-        <v>30.049000024795532</v>
+        <v>30.06599998474121</v>
       </c>
       <c r="C11" t="s">
         <v>33</v>
@@ -721,7 +721,7 @@
         <v>35</v>
       </c>
       <c r="B12">
-        <v>30.031999826431274</v>
+        <v>30.051000118255615</v>
       </c>
       <c r="C12" t="s">
         <v>36</v>

</xml_diff>